<commit_message>
11th MD Single Ticker Enhancement
</commit_message>
<xml_diff>
--- a/Reports/ZacksRank/TanzyToInvest.xlsx
+++ b/Reports/ZacksRank/TanzyToInvest.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i852841/_Codes/_Personal/StockRankingCrawler/Reports/ZacksRank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{2A68826B-7E83-0C4A-B48D-626FEF9DF880}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DB2955-8835-3F45-BA75-3FF2539D42D8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="19560" windowWidth="33600" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="data" r:id="rId1" sheetId="1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="197">
   <si>
     <t>ETSY</t>
   </si>
@@ -523,9 +523,6 @@
     <t>Hold       ($66.73)</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Jun_27</t>
   </si>
   <si>
@@ -557,14 +554,70 @@
   </si>
   <si>
     <t>Hold       ($65.46)</t>
+  </si>
+  <si>
+    <t>Jun_28</t>
+  </si>
+  <si>
+    <t>Buy        ($40.79)</t>
+  </si>
+  <si>
+    <t>Hold       ($24.78)</t>
+  </si>
+  <si>
+    <t>Hold       ($10.27)</t>
+  </si>
+  <si>
+    <t>Hold       ($68.60)</t>
+  </si>
+  <si>
+    <t>Hold       ($22.01)</t>
+  </si>
+  <si>
+    <t>Hold       ($33.00)</t>
+  </si>
+  <si>
+    <t>UN         ($0.29)</t>
+  </si>
+  <si>
+    <t>Buy        ($35.30)</t>
+  </si>
+  <si>
+    <t>Hold       ($25.36)</t>
+  </si>
+  <si>
+    <t>Hold       ($64.41)</t>
+  </si>
+  <si>
+    <t>AOI</t>
+  </si>
+  <si>
+    <t>UN         ($16.05)</t>
+  </si>
+  <si>
+    <t>HCLP</t>
+  </si>
+  <si>
+    <t>StrongBuy  ($11.70)</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Hold       ($15.94)</t>
+  </si>
+  <si>
+    <t>HZNP</t>
+  </si>
+  <si>
+    <t>Hold       ($16.04)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -572,8 +625,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -595,6 +655,12 @@
         <fgColor indexed="42"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -606,83 +672,96 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="81">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -699,10 +778,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -737,7 +816,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -789,7 +868,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -900,21 +979,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -931,7 +1010,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -983,755 +1062,796 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="13.6640625" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="13.6640625" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="13.6640625" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" width="13.6640625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" width="10.0" collapsed="false"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="25" width="16" customWidth="1" collapsed="1"/>
+    <col min="26" max="29" width="13.6640625" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C1" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" t="s">
         <v>164</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" t="s">
         <v>145</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" t="s">
         <v>137</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" t="s">
         <v>129</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" t="s">
         <v>118</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" t="s">
         <v>108</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L1" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="M1" t="s">
         <v>96</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="N1" t="s">
         <v>88</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="O1" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="P1" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="Q1" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="R1" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="S1" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="T1" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="U1" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="V1" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="X1" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="Y1" t="s">
         <v>12</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Z1" t="s">
         <v>10</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="AA1" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AB1" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AC1" t="s">
         <v>4</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AD1" t="s">
         <v>1</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AE1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="48" t="s">
+      <c r="B2" s="68" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="E2" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="F2" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="G2" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" t="s">
         <v>109</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="K2" t="s">
         <v>109</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="L2" t="s">
         <v>99</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="M2" t="s">
         <v>89</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="N2" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="O2" t="s">
         <v>67</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="P2" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="Q2" t="s">
         <v>53</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="R2" t="s">
         <v>46</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="S2" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="T2" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="U2" t="s">
         <v>31</v>
       </c>
-      <c r="U2" s="0" t="s">
+      <c r="V2" t="s">
         <v>26</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="W2" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="X2" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="0" t="s">
+      <c r="Y2" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="0" t="s">
+      <c r="Z2" t="s">
         <v>11</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AA2" s="0" t="s">
+      <c r="AB2" t="s">
         <v>5</v>
       </c>
-      <c r="AB2" s="0" t="s">
+      <c r="AC2" t="s">
         <v>5</v>
       </c>
-      <c r="AC2" s="0" t="s">
+      <c r="AD2" t="s">
         <v>3</v>
       </c>
-      <c r="AD2" s="0" t="s">
+      <c r="AE2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="59" t="s">
-        <v>170</v>
-      </c>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="69" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="49" t="s">
         <v>155</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="E3" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="F3" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="G3" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="J3" t="s">
         <v>110</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="K3" t="s">
         <v>110</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="L3" t="s">
         <v>100</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="M3" t="s">
         <v>90</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="N3" t="s">
         <v>90</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="O3" t="s">
         <v>68</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="P3" t="s">
         <v>60</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="Q3" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="R3" t="s">
         <v>47</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="S3" t="s">
         <v>39</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="T3" t="s">
         <v>39</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="U3" t="s">
         <v>32</v>
       </c>
-      <c r="U3" s="0" t="s">
+      <c r="V3" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="0" t="s">
+      <c r="W3" t="s">
         <v>21</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="X3" t="s">
         <v>16</v>
       </c>
-      <c r="X3" s="0" t="s">
+      <c r="Y3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="60" t="s">
-        <v>171</v>
-      </c>
-      <c r="C4" s="50" t="s">
+      <c r="B4" s="70" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="60" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="E4" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="F4" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="G4" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="H4" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="J4" t="s">
         <v>111</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="K4" t="s">
         <v>111</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="L4" t="s">
         <v>101</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="M4" t="s">
         <v>91</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="N4" t="s">
         <v>91</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="O4" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="P4" t="s">
         <v>61</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="Q4" t="s">
         <v>55</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="R4" t="s">
         <v>48</v>
       </c>
-      <c r="R4" s="0" t="s">
+      <c r="S4" t="s">
         <v>28</v>
       </c>
-      <c r="S4" s="0" t="s">
+      <c r="T4" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="0" t="s">
+      <c r="U4" t="s">
         <v>33</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="0" t="s">
+      <c r="W4" t="s">
         <v>22</v>
       </c>
-      <c r="W4" s="0" t="s">
+      <c r="X4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="61" t="s">
-        <v>172</v>
-      </c>
-      <c r="C5" s="51" t="s">
+      <c r="B5" s="71" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" s="51" t="s">
         <v>156</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="E5" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="F5" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="G5" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="H5" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="J5" t="s">
         <v>112</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="K5" t="s">
         <v>112</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="L5" t="s">
         <v>102</v>
       </c>
-      <c r="L5" s="0" t="s">
+      <c r="M5" t="s">
         <v>92</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="N5" t="s">
         <v>92</v>
       </c>
-      <c r="N5" s="0" t="s">
+      <c r="O5" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="0" t="s">
+      <c r="P5" t="s">
         <v>62</v>
       </c>
-      <c r="P5" s="0" t="s">
+      <c r="Q5" t="s">
         <v>56</v>
       </c>
-      <c r="Q5" s="0" t="s">
+      <c r="R5" t="s">
         <v>49</v>
       </c>
-      <c r="R5" s="0" t="s">
+      <c r="S5" t="s">
         <v>40</v>
       </c>
-      <c r="S5" s="0" t="s">
+      <c r="T5" t="s">
         <v>40</v>
       </c>
-      <c r="T5" s="0" t="s">
+      <c r="U5" t="s">
         <v>34</v>
       </c>
-      <c r="U5" s="0" t="s">
+      <c r="V5" t="s">
         <v>29</v>
       </c>
-      <c r="V5" s="0" t="s">
+      <c r="W5" t="s">
         <v>23</v>
       </c>
-      <c r="W5" s="0" t="s">
+      <c r="X5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="62" t="s">
-        <v>173</v>
-      </c>
-      <c r="C6" s="52" t="s">
+      <c r="B6" s="72" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" s="62" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="E6" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="F6" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="G6" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="H6" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="J6" t="s">
         <v>113</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="K6" t="s">
         <v>113</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="L6" t="s">
         <v>103</v>
       </c>
-      <c r="L6" s="0" t="s">
+      <c r="M6" t="s">
         <v>71</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="N6" t="s">
         <v>71</v>
       </c>
-      <c r="N6" s="0" t="s">
+      <c r="O6" t="s">
         <v>71</v>
       </c>
-      <c r="O6" s="0" t="s">
+      <c r="P6" t="s">
         <v>63</v>
       </c>
-      <c r="P6" s="0" t="s">
+      <c r="Q6" t="s">
         <v>57</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="R6" t="s">
         <v>50</v>
       </c>
-      <c r="R6" s="0" t="s">
+      <c r="S6" t="s">
         <v>41</v>
       </c>
-      <c r="S6" s="0" t="s">
+      <c r="T6" t="s">
         <v>41</v>
       </c>
-      <c r="T6" s="0" t="s">
+      <c r="U6" t="s">
         <v>35</v>
       </c>
-      <c r="U6" s="0" t="s">
+      <c r="V6" t="s">
         <v>30</v>
       </c>
-      <c r="V6" s="0" t="s">
+      <c r="W6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="63" t="s">
-        <v>174</v>
-      </c>
-      <c r="C7" s="53" t="s">
+      <c r="B7" s="73" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" s="53" t="s">
         <v>157</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="E7" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="F7" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="G7" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="H7" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="I7" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="J7" t="s">
         <v>114</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="K7" t="s">
         <v>114</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="L7" t="s">
         <v>104</v>
       </c>
-      <c r="L7" s="0" t="s">
+      <c r="M7" t="s">
         <v>93</v>
       </c>
-      <c r="M7" s="0" t="s">
+      <c r="N7" t="s">
         <v>93</v>
       </c>
-      <c r="N7" s="0" t="s">
+      <c r="O7" t="s">
         <v>72</v>
       </c>
-      <c r="O7" s="0" t="s">
+      <c r="P7" t="s">
         <v>64</v>
       </c>
-      <c r="P7" s="0" t="s">
+      <c r="Q7" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="R7" t="s">
         <v>51</v>
       </c>
-      <c r="R7" s="0" t="s">
+      <c r="S7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="64" t="s">
-        <v>175</v>
-      </c>
-      <c r="C8" s="54" t="s">
+      <c r="B8" s="74" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" s="64" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" s="54" t="s">
         <v>158</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="E8" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="F8" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="G8" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="H8" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="I8" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="J8" t="s">
         <v>115</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="K8" t="s">
         <v>115</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="L8" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="0" t="s">
+      <c r="M8" t="s">
         <v>94</v>
       </c>
-      <c r="M8" s="0" t="s">
+      <c r="N8" t="s">
         <v>94</v>
       </c>
-      <c r="N8" s="0" t="s">
+      <c r="O8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="65" t="s">
-        <v>176</v>
-      </c>
-      <c r="C9" s="55" t="s">
+      <c r="B9" s="75" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="65" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" s="55" t="s">
         <v>159</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="E9" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="F9" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="G9" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="H9" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="I9" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="J9" t="s">
         <v>116</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="K9" t="s">
         <v>116</v>
       </c>
-      <c r="K9" s="0" t="s">
+      <c r="L9" t="s">
         <v>106</v>
       </c>
-      <c r="L9" s="0" t="s">
+      <c r="M9" t="s">
         <v>95</v>
       </c>
-      <c r="M9" s="0" t="s">
+      <c r="N9" t="s">
         <v>95</v>
       </c>
-      <c r="N9" s="0" t="s">
+      <c r="O9" t="s">
         <v>75</v>
       </c>
-      <c r="O9" s="0" t="s">
+      <c r="P9" t="s">
         <v>76</v>
       </c>
-      <c r="P9" s="0" t="s">
+      <c r="Q9" t="s">
         <v>77</v>
       </c>
-      <c r="Q9" s="0" t="s">
+      <c r="R9" t="s">
         <v>78</v>
       </c>
-      <c r="R9" s="0" t="s">
+      <c r="S9" t="s">
         <v>79</v>
       </c>
-      <c r="S9" s="0" t="s">
+      <c r="T9" t="s">
         <v>79</v>
       </c>
-      <c r="T9" s="0" t="s">
+      <c r="U9" t="s">
         <v>80</v>
       </c>
-      <c r="U9" s="0" t="s">
+      <c r="V9" t="s">
         <v>81</v>
       </c>
-      <c r="V9" s="0" t="s">
+      <c r="W9" t="s">
         <v>82</v>
       </c>
-      <c r="W9" s="0" t="s">
+      <c r="X9" t="s">
         <v>83</v>
       </c>
-      <c r="X9" s="0" t="s">
+      <c r="Y9" t="s">
         <v>84</v>
       </c>
-      <c r="Y9" s="0" t="s">
+      <c r="Z9" t="s">
         <v>85</v>
       </c>
-      <c r="Z9" s="0" t="s">
+      <c r="AA9" t="s">
         <v>86</v>
       </c>
-      <c r="AA9" s="0" t="s">
+      <c r="AB9" t="s">
         <v>86</v>
       </c>
-      <c r="AB9" s="0" t="s">
+      <c r="AC9" t="s">
         <v>87</v>
       </c>
-      <c r="AC9" s="0" t="s">
+      <c r="AD9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="66" t="s">
-        <v>177</v>
-      </c>
-      <c r="C10" s="56" t="s">
+      <c r="B10" s="76" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="D10" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="E10" s="47" t="s">
         <v>160</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="F10" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="G10" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="H10" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="I10" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="J10" t="s">
         <v>117</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="K10" t="s">
         <v>117</v>
       </c>
-      <c r="K10" s="57" t="s">
+      <c r="L10" s="57" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="67" t="s">
-        <v>178</v>
-      </c>
-      <c r="C11" s="57" t="s">
+      <c r="B11" s="77" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" s="67" t="s">
+        <v>177</v>
+      </c>
+      <c r="D11" s="57" t="s">
         <v>166</v>
       </c>
-      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" s="78" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A13" s="80" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" s="79" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>193</v>
+      </c>
+      <c r="B14" s="78" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B15" s="78" t="s">
+        <v>196</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>